<commit_message>
[STABILIZATION + EXECUTION] added feature for extent reporting
</commit_message>
<xml_diff>
--- a/Documents/HowToExecute, Approach, Defects - BuggyCarsRating.xlsx
+++ b/Documents/HowToExecute, Approach, Defects - BuggyCarsRating.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karyll Urma\OneDrive\Documents\GOALS\Westpac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karyll Urma\OneDrive\Documents\GitHub\Test.BuggyCarsRating\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1378A7-14B0-4766-801B-2E662ED662F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141AFA09-DE14-4CEC-80E4-C712E655A06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-10470" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A5DF0929-27CD-4336-A6FB-AD82504CCBFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{A5DF0929-27CD-4336-A6FB-AD82504CCBFA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Automation Approach" sheetId="3" r:id="rId1"/>
-    <sheet name="How To " sheetId="2" r:id="rId2"/>
+    <sheet name="Approach" sheetId="3" r:id="rId1"/>
+    <sheet name="How To" sheetId="2" r:id="rId2"/>
     <sheet name="Defects" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Defect Id</t>
   </si>
@@ -248,24 +248,6 @@
     <t>Step 5: All set to run scripts.</t>
   </si>
   <si>
-    <t xml:space="preserve">Framework: </t>
-  </si>
-  <si>
-    <t>.Net 5.0</t>
-  </si>
-  <si>
-    <t>Test Framework:</t>
-  </si>
-  <si>
-    <t>Nunit</t>
-  </si>
-  <si>
-    <t>Model:</t>
-  </si>
-  <si>
-    <t>BDD using Specflow</t>
-  </si>
-  <si>
     <t>The automation framework is designed using the following specifications below:</t>
   </si>
   <si>
@@ -277,6 +259,18 @@
   </si>
   <si>
     <t>A set of libraries such as Helpers, Base, Contexts, Runsettings/Config  are created to develop the framework on top of the basics: Features, Pages, Hooks and Steps.</t>
+  </si>
+  <si>
+    <t>Framework design Model:</t>
+  </si>
+  <si>
+    <t>Behavioral Driven Development - Specflow</t>
+  </si>
+  <si>
+    <t>.Net 5.0, C#, Nunit, Gherkin</t>
+  </si>
+  <si>
+    <t>Technology/Framework:</t>
   </si>
 </sst>
 </file>
@@ -474,55 +468,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>97449</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C94602A-87B8-40A6-8DEA-122345611B4C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2857500"/>
-          <a:ext cx="5448300" cy="1811949"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1044,76 +989,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8791A2AE-35E2-45EA-819A-590332B5EC91}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
+      <c r="A5" s="7"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="14" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>58</v>
+      <c r="A7" s="15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1122,7 +1055,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1132,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>